<commit_message>
feat: add host function
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
+++ b/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
@@ -2675,7 +2675,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2920,13 +2920,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3895,225 +3889,225 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.1333333333333" style="105" customWidth="1"/>
-    <col min="2" max="2" width="9" style="105"/>
-    <col min="3" max="3" width="27.7333333333333" style="105" customWidth="1"/>
-    <col min="4" max="4" width="4.75833333333333" style="105" customWidth="1"/>
-    <col min="5" max="5" width="17.1333333333333" style="105" customWidth="1"/>
-    <col min="6" max="6" width="9" style="105"/>
-    <col min="7" max="7" width="29.525" style="105" customWidth="1"/>
-    <col min="8" max="8" width="42.5" style="105" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="105"/>
+    <col min="1" max="1" width="17.1333333333333" style="103" customWidth="1"/>
+    <col min="2" max="2" width="9" style="103"/>
+    <col min="3" max="3" width="27.7333333333333" style="103" customWidth="1"/>
+    <col min="4" max="4" width="4.75833333333333" style="103" customWidth="1"/>
+    <col min="5" max="5" width="17.1333333333333" style="103" customWidth="1"/>
+    <col min="6" max="6" width="9" style="103"/>
+    <col min="7" max="7" width="29.525" style="103" customWidth="1"/>
+    <col min="8" max="8" width="42.5" style="103" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="103"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="113" t="s">
+      <c r="D1" s="112"/>
+      <c r="E1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="111" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="115" t="s">
+      <c r="E2" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115" t="s">
+      <c r="G2" s="113"/>
+      <c r="H2" s="113" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="27" spans="1:8">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="115" t="s">
+      <c r="F3" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="115"/>
-      <c r="H3" s="116" t="s">
+      <c r="G3" s="113"/>
+      <c r="H3" s="114" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" ht="40.5" spans="1:8">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="115" t="s">
+      <c r="E4" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="115" t="s">
+      <c r="F4" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="115" t="s">
+      <c r="G4" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="116" t="s">
+      <c r="H4" s="114" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="115"/>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="E5" s="115" t="s">
+      <c r="A5" s="113"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="113"/>
+      <c r="E5" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="115" t="s">
+      <c r="G5" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="115"/>
+      <c r="H5" s="113"/>
     </row>
     <row r="6" ht="54" spans="1:8">
-      <c r="A6" s="115"/>
-      <c r="B6" s="115"/>
-      <c r="C6" s="115"/>
-      <c r="E6" s="115" t="s">
+      <c r="A6" s="113"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="113"/>
+      <c r="E6" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="115" t="s">
+      <c r="F6" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="116" t="s">
+      <c r="G6" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="116" t="s">
+      <c r="H6" s="114" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="115" t="s">
+      <c r="E7" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="115" t="s">
+      <c r="F7" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="115" t="s">
+      <c r="G7" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="116" t="s">
+      <c r="H7" s="114" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="115" t="s">
+      <c r="A8" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="115" t="s">
+      <c r="C8" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="115" t="s">
+      <c r="E8" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="115" t="s">
+      <c r="F8" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="116" t="s">
+      <c r="G8" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="116" t="s">
+      <c r="H8" s="114" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="115" t="s">
+      <c r="A9" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="115" t="s">
+      <c r="B9" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="115" t="s">
+      <c r="E9" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="115" t="s">
+      <c r="F9" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="115" t="s">
+      <c r="G9" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="115"/>
+      <c r="H9" s="113"/>
     </row>
     <row r="10" ht="27" spans="1:8">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="115" t="s">
+      <c r="B10" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="115" t="s">
+      <c r="C10" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="115" t="s">
+      <c r="E10" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="115" t="s">
+      <c r="F10" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="115" t="s">
+      <c r="G10" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="116" t="s">
+      <c r="H10" s="114" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4859,478 +4853,478 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="15.25" style="105" customWidth="1"/>
-    <col min="2" max="2" width="30.6333333333333" style="105" customWidth="1"/>
-    <col min="3" max="3" width="25.6333333333333" style="105" customWidth="1"/>
-    <col min="4" max="4" width="11.1333333333333" style="105" customWidth="1"/>
-    <col min="5" max="5" width="9.875" style="105" customWidth="1"/>
-    <col min="6" max="6" width="32.625" style="105" customWidth="1"/>
-    <col min="7" max="7" width="17.8833333333333" style="105" customWidth="1"/>
-    <col min="8" max="8" width="28.25" style="105" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="105"/>
+    <col min="1" max="1" width="15.25" style="103" customWidth="1"/>
+    <col min="2" max="2" width="30.6333333333333" style="103" customWidth="1"/>
+    <col min="3" max="3" width="25.6333333333333" style="103" customWidth="1"/>
+    <col min="4" max="4" width="11.1333333333333" style="103" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="103" customWidth="1"/>
+    <col min="6" max="6" width="32.625" style="103" customWidth="1"/>
+    <col min="7" max="7" width="17.8833333333333" style="103" customWidth="1"/>
+    <col min="8" max="8" width="28.25" style="103" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="103"/>
   </cols>
   <sheetData>
-    <row r="1" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A1" s="97" t="s">
+    <row r="1" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A1" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="95" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A2" s="98">
+    <row r="2" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A2" s="96">
         <v>1001</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="98">
+      <c r="D2" s="96">
         <v>1</v>
       </c>
-      <c r="E2" s="98">
+      <c r="E2" s="96">
         <v>501</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="98" t="s">
+      <c r="G2" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="98" t="s">
+      <c r="H2" s="96" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A3" s="98">
+    <row r="3" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A3" s="96">
         <v>1002</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="98">
+      <c r="D3" s="96">
         <v>2</v>
       </c>
-      <c r="E3" s="98">
+      <c r="E3" s="96">
         <v>502</v>
       </c>
-      <c r="F3" s="98" t="s">
+      <c r="F3" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="98" t="s">
+      <c r="G3" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="96" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A4" s="107">
+    <row r="4" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A4" s="105">
         <v>1003</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="107">
+      <c r="D4" s="105">
         <v>3</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="96">
         <v>503</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="98" t="s">
+      <c r="H4" s="96" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A5" s="109"/>
-      <c r="B5" s="109"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="98">
+    <row r="5" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A5" s="107"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="96">
         <v>516</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="96" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A6" s="111"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="98">
+    <row r="6" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A6" s="109"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="96">
         <v>517</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="98" t="s">
+      <c r="G6" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="98" t="s">
+      <c r="H6" s="96" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A7" s="109">
+    <row r="7" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A7" s="107">
         <v>1004</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="109">
+      <c r="D7" s="107">
         <v>4</v>
       </c>
-      <c r="E7" s="98">
+      <c r="E7" s="96">
         <v>504</v>
       </c>
-      <c r="F7" s="98" t="s">
+      <c r="F7" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="98" t="s">
+      <c r="G7" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="96" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A8" s="109"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="98">
+    <row r="8" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="96">
         <v>527</v>
       </c>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="98" t="s">
+      <c r="G8" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="98" t="s">
+      <c r="H8" s="96" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A9" s="111"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="98">
+    <row r="9" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A9" s="109"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="96">
         <v>528</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="98" t="s">
+      <c r="G9" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="98" t="s">
+      <c r="H9" s="96" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A10" s="107">
+    <row r="10" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A10" s="105">
         <v>1005</v>
       </c>
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="107">
+      <c r="D10" s="105">
         <v>5</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="96">
         <v>505</v>
       </c>
-      <c r="F10" s="98" t="s">
+      <c r="F10" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="98" t="s">
+      <c r="G10" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="98" t="s">
+      <c r="H10" s="96" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A11" s="109"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="98">
+    <row r="11" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A11" s="107"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="96">
         <v>506</v>
       </c>
-      <c r="F11" s="98" t="s">
+      <c r="F11" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="98" t="s">
+      <c r="G11" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="98" t="s">
+      <c r="H11" s="96" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A12" s="109"/>
-      <c r="B12" s="109"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="98">
+    <row r="12" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A12" s="107"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="96">
         <v>507</v>
       </c>
-      <c r="F12" s="98" t="s">
+      <c r="F12" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="98" t="s">
+      <c r="G12" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="98" t="s">
+      <c r="H12" s="96" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A13" s="109"/>
-      <c r="B13" s="109"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="98">
+    <row r="13" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A13" s="107"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="96">
         <v>508</v>
       </c>
-      <c r="F13" s="98" t="s">
+      <c r="F13" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="98" t="s">
+      <c r="G13" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="98" t="s">
+      <c r="H13" s="96" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A14" s="111"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="112"/>
-      <c r="D14" s="98">
+    <row r="14" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A14" s="109"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="96">
         <v>6</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="96">
         <v>509</v>
       </c>
-      <c r="F14" s="98" t="s">
+      <c r="F14" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="G14" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="98" t="s">
+      <c r="H14" s="96" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A15" s="107">
+    <row r="15" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A15" s="105">
         <v>1006</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="105" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="106" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="107">
+      <c r="D15" s="105">
         <v>7</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="96">
         <v>506</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F15" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="98" t="s">
+      <c r="H15" s="96" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A16" s="109"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="98">
+    <row r="16" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A16" s="107"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="96">
         <v>508</v>
       </c>
-      <c r="F16" s="98" t="s">
+      <c r="F16" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="98" t="s">
+      <c r="G16" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="98" t="s">
+      <c r="H16" s="96" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A17" s="111"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="98">
+    <row r="17" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A17" s="109"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="96">
         <v>6</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="96">
         <v>509</v>
       </c>
-      <c r="F17" s="98" t="s">
+      <c r="F17" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="98" t="s">
+      <c r="G17" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="98" t="s">
+      <c r="H17" s="96" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A18" s="107">
+    <row r="18" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A18" s="105">
         <v>1007</v>
       </c>
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="107">
+      <c r="D18" s="105">
         <v>8</v>
       </c>
-      <c r="E18" s="98">
+      <c r="E18" s="96">
         <v>505</v>
       </c>
-      <c r="F18" s="98" t="s">
+      <c r="F18" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="98" t="s">
+      <c r="H18" s="96" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A19" s="109"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="98">
+    <row r="19" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A19" s="107"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="96">
         <v>523</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="98" t="s">
+      <c r="G19" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="98" t="s">
+      <c r="H19" s="96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" s="105" customFormat="1" ht="18.75" spans="1:8">
-      <c r="A20" s="109"/>
-      <c r="B20" s="109"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="98">
+    <row r="20" s="103" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A20" s="107"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="96">
         <v>524</v>
       </c>
-      <c r="F20" s="98" t="s">
+      <c r="F20" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="98" t="s">
+      <c r="G20" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="98" t="s">
+      <c r="H20" s="96" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="21" ht="18.75" spans="1:8">
-      <c r="A21" s="109"/>
-      <c r="B21" s="109"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="98">
+      <c r="A21" s="107"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="96">
         <v>525</v>
       </c>
-      <c r="F21" s="98" t="s">
+      <c r="F21" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="98" t="s">
+      <c r="G21" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="98" t="s">
+      <c r="H21" s="96" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="22" ht="18.75" spans="1:8">
-      <c r="A22" s="111"/>
-      <c r="B22" s="111"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="98">
+      <c r="A22" s="109"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="96">
         <v>526</v>
       </c>
-      <c r="F22" s="98" t="s">
+      <c r="F22" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="98" t="s">
+      <c r="G22" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="96" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5375,7 +5369,7 @@
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="29.3833333333333" customWidth="1"/>
-    <col min="3" max="3" width="5.38333333333333" style="100" customWidth="1"/>
+    <col min="3" max="3" width="5.38333333333333" style="98" customWidth="1"/>
     <col min="4" max="4" width="29.3833333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5391,10 +5385,10 @@
       </c>
     </row>
     <row r="2" ht="16.5" spans="1:3">
-      <c r="A2" s="101">
+      <c r="A2" s="99">
         <v>0</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="100" t="s">
         <v>104</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -5402,16 +5396,16 @@
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:4">
-      <c r="A3" s="101">
+      <c r="A3" s="99">
         <v>1</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="101" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="102" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5419,13 +5413,13 @@
       <c r="A4" s="75">
         <v>10</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="100" t="s">
         <v>108</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="104"/>
+      <c r="D4" s="102"/>
     </row>
     <row r="5" ht="16.5" spans="1:4">
       <c r="A5" s="75">
@@ -5437,7 +5431,7 @@
       <c r="C5" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="104"/>
+      <c r="D5" s="102"/>
     </row>
     <row r="6" ht="16.5" spans="1:4">
       <c r="A6" s="75">
@@ -5449,7 +5443,7 @@
       <c r="C6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="104"/>
+      <c r="D6" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5473,342 +5467,342 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.13333333333333" style="96" customWidth="1"/>
-    <col min="2" max="2" width="41" style="96" customWidth="1"/>
-    <col min="3" max="3" width="21.3833333333333" style="96" customWidth="1"/>
-    <col min="4" max="4" width="25.1333333333333" style="96" customWidth="1"/>
-    <col min="5" max="5" width="36" style="96" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="96"/>
+    <col min="1" max="1" width="9.13333333333333" style="94" customWidth="1"/>
+    <col min="2" max="2" width="41" style="94" customWidth="1"/>
+    <col min="3" max="3" width="21.3833333333333" style="94" customWidth="1"/>
+    <col min="4" max="4" width="25.1333333333333" style="94" customWidth="1"/>
+    <col min="5" max="5" width="36" style="94" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="94"/>
   </cols>
   <sheetData>
-    <row r="1" s="96" customFormat="1" spans="1:5">
-      <c r="A1" s="97" t="s">
+    <row r="1" s="94" customFormat="1" spans="1:5">
+      <c r="A1" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="95" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" s="96" customFormat="1" ht="37.5" spans="1:5">
-      <c r="A2" s="98">
+    <row r="2" s="94" customFormat="1" ht="37.5" spans="1:5">
+      <c r="A2" s="96">
         <v>501</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="99" t="s">
+      <c r="E2" s="97" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" s="96" customFormat="1" ht="112.5" spans="1:5">
-      <c r="A3" s="98">
+    <row r="3" s="94" customFormat="1" ht="112.5" spans="1:5">
+      <c r="A3" s="96">
         <v>502</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="99" t="s">
+      <c r="E3" s="97" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="98">
+      <c r="A4" s="96">
         <v>503</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="99"/>
+      <c r="E4" s="97"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="98">
+      <c r="A5" s="96">
         <v>504</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="99"/>
+      <c r="E5" s="97"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="98">
+      <c r="A6" s="96">
         <v>505</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="98" t="s">
+      <c r="D6" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="99"/>
+      <c r="E6" s="97"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="98">
+      <c r="A7" s="96">
         <v>506</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="98" t="s">
+      <c r="D7" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="99"/>
+      <c r="E7" s="97"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="98">
+      <c r="A8" s="96">
         <v>507</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="98" t="s">
+      <c r="C8" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="96" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="99"/>
+      <c r="E8" s="97"/>
     </row>
     <row r="9" ht="75" spans="1:5">
-      <c r="A9" s="98">
+      <c r="A9" s="96">
         <v>508</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="98" t="s">
+      <c r="C9" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="99" t="s">
+      <c r="E9" s="97" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="98">
+      <c r="A10" s="96">
         <v>509</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="98" t="s">
+      <c r="D10" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="99"/>
+      <c r="E10" s="97"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="98">
+      <c r="A11" s="96">
         <v>511</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="98" t="s">
+      <c r="C11" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="99"/>
+      <c r="E11" s="97"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="98">
+      <c r="A12" s="96">
         <v>512</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="98" t="s">
+      <c r="C12" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="96" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="99"/>
+      <c r="E12" s="97"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="98">
+      <c r="A13" s="96">
         <v>513</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="98" t="s">
+      <c r="C13" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="99"/>
+      <c r="E13" s="97"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="98">
+      <c r="A14" s="96">
         <v>514</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="98" t="s">
+      <c r="C14" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="E14" s="99"/>
+      <c r="E14" s="97"/>
     </row>
     <row r="15" ht="56.25" spans="1:5">
-      <c r="A15" s="98">
+      <c r="A15" s="96">
         <v>516</v>
       </c>
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="98" t="s">
+      <c r="D15" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="99" t="s">
+      <c r="E15" s="97" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="98">
+      <c r="A16" s="96">
         <v>517</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="99"/>
+      <c r="E16" s="97"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="98">
+      <c r="A17" s="96">
         <v>523</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="98" t="s">
+      <c r="C17" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="98" t="s">
+      <c r="D17" s="96" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="99"/>
+      <c r="E17" s="97"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="98">
+      <c r="A18" s="96">
         <v>524</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="98" t="s">
+      <c r="C18" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="99"/>
+      <c r="E18" s="97"/>
     </row>
     <row r="19" ht="37.5" spans="1:5">
-      <c r="A19" s="98">
+      <c r="A19" s="96">
         <v>525</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="98" t="s">
+      <c r="C19" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="99" t="s">
+      <c r="E19" s="97" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="20" ht="37.5" spans="1:5">
-      <c r="A20" s="98">
+      <c r="A20" s="96">
         <v>526</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="98" t="s">
+      <c r="C20" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="96" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="99" t="s">
+      <c r="E20" s="97" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="98">
+      <c r="A21" s="96">
         <v>529</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="99"/>
+      <c r="E21" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5836,46 +5830,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="90" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="40.5" spans="1:3">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="91" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="92" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="91" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="93" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="91" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="93" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="93" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5892,9 +5886,9 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5923,1948 +5917,1948 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A2" s="83" t="s">
+    <row r="2" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A2" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85"/>
-    </row>
-    <row r="3" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A3" s="86" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="83"/>
+    </row>
+    <row r="3" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A3" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="84" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A4" s="83" t="s">
+    <row r="4" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A4" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85"/>
-    </row>
-    <row r="5" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A5" s="84" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="83"/>
+    </row>
+    <row r="5" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A5" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="85" t="s">
+      <c r="C5" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A6" s="83" t="s">
+    <row r="6" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A6" s="82" t="s">
         <v>156</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="85"/>
-    </row>
-    <row r="7" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A7" s="84" t="s">
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="83"/>
+    </row>
+    <row r="7" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A7" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="85" t="s">
+      <c r="C7" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A8" s="83" t="s">
+    <row r="8" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A8" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="85"/>
-    </row>
-    <row r="9" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A9" s="84" t="s">
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="83"/>
+    </row>
+    <row r="9" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A9" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="85" t="s">
+      <c r="C9" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A10" s="83" t="s">
+    <row r="10" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A10" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="85"/>
-    </row>
-    <row r="11" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A11" s="86" t="s">
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="83"/>
+    </row>
+    <row r="11" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A11" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="84" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="87" t="s">
+      <c r="E11" s="85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="12" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A12" s="86" t="s">
+    <row r="12" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A12" s="84" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="84" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E12" s="87" t="s">
+      <c r="E12" s="85" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A13" s="86" t="s">
+    <row r="13" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A13" s="84" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="D13" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="87" t="s">
+      <c r="E13" s="85" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A14" s="86" t="s">
+    <row r="14" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A14" s="84" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="87" t="s">
+      <c r="E14" s="85" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="15" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A15" s="84" t="s">
+    <row r="15" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A15" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="85" t="s">
+      <c r="C15" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="83" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A16" s="84" t="s">
+    <row r="16" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A16" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E16" s="85" t="s">
+      <c r="C16" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A17" s="84" t="s">
+    <row r="17" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A17" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="80" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D17" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="85" t="s">
+      <c r="C17" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A18" s="84" t="s">
+    <row r="18" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A18" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="B18" s="84" t="s">
+      <c r="B18" s="80" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E18" s="85" t="s">
+      <c r="C18" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A19" s="83" t="s">
+    <row r="19" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A19" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="85"/>
-    </row>
-    <row r="20" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A20" s="84" t="s">
+      <c r="B19" s="80"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="83"/>
+    </row>
+    <row r="20" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A20" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="85" t="s">
+      <c r="C20" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="83" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="21" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A21" s="84" t="s">
+    <row r="21" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A21" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="80" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E21" s="85" t="s">
+      <c r="C21" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="22" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A22" s="84" t="s">
+    <row r="22" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A22" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="80" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="85" t="s">
+      <c r="C22" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A23" s="86" t="s">
+    <row r="23" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A23" s="84" t="s">
         <v>179</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="84" t="s">
         <v>180</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E23" s="87" t="s">
+      <c r="E23" s="85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A24" s="83" t="s">
+    <row r="24" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A24" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="85"/>
-    </row>
-    <row r="25" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A25" s="84" t="s">
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="83"/>
+    </row>
+    <row r="25" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A25" s="80" t="s">
         <v>181</v>
       </c>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="80" t="s">
         <v>182</v>
       </c>
-      <c r="C25" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D25" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="85" t="s">
+      <c r="C25" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="83" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A26" s="84" t="s">
+    <row r="26" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A26" s="80" t="s">
         <v>183</v>
       </c>
-      <c r="B26" s="84" t="s">
+      <c r="B26" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" s="85" t="s">
+      <c r="C26" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="27" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A27" s="84" t="s">
+    <row r="27" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A27" s="80" t="s">
         <v>185</v>
       </c>
-      <c r="B27" s="84" t="s">
+      <c r="B27" s="80" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="84" t="s">
+      <c r="C27" s="80" t="s">
         <v>147</v>
       </c>
-      <c r="D27" s="84" t="s">
+      <c r="D27" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="E27" s="85" t="s">
+      <c r="E27" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A28" s="86" t="s">
+    <row r="28" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A28" s="84" t="s">
         <v>187</v>
       </c>
-      <c r="B28" s="86" t="s">
+      <c r="B28" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="86" t="s">
+      <c r="D28" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="87" t="s">
+      <c r="E28" s="85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A29" s="83" t="s">
+    <row r="29" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A29" s="82" t="s">
         <v>189</v>
       </c>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="85"/>
-    </row>
-    <row r="30" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A30" s="84" t="s">
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="83"/>
+    </row>
+    <row r="30" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A30" s="80" t="s">
         <v>190</v>
       </c>
-      <c r="B30" s="84" t="s">
+      <c r="B30" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="C30" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="85" t="s">
+      <c r="C30" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="83" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="31" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A31" s="84" t="s">
+    <row r="31" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A31" s="80" t="s">
         <v>192</v>
       </c>
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="C31" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="85" t="s">
+      <c r="C31" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="32" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A32" s="84" t="s">
+    <row r="32" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A32" s="80" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="80" t="s">
         <v>194</v>
       </c>
-      <c r="C32" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32" s="85" t="s">
+      <c r="C32" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="33" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A33" s="84" t="s">
+    <row r="33" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A33" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="B33" s="84" t="s">
+      <c r="B33" s="80" t="s">
         <v>196</v>
       </c>
-      <c r="C33" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D33" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E33" s="85" t="s">
+      <c r="C33" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="34" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A34" s="84" t="s">
+    <row r="34" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A34" s="80" t="s">
         <v>197</v>
       </c>
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D34" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E34" s="85" t="s">
+      <c r="C34" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="35" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A35" s="84" t="s">
+    <row r="35" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A35" s="80" t="s">
         <v>198</v>
       </c>
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="80" t="s">
         <v>199</v>
       </c>
-      <c r="C35" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D35" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="85" t="s">
+      <c r="C35" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A36" s="84" t="s">
+    <row r="36" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A36" s="80" t="s">
         <v>200</v>
       </c>
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="C36" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D36" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" s="85" t="s">
+      <c r="C36" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A37" s="84" t="s">
+    <row r="37" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A37" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="80" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D37" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E37" s="85" t="s">
+      <c r="C37" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A38" s="84" t="s">
+    <row r="38" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A38" s="80" t="s">
         <v>204</v>
       </c>
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="80" t="s">
         <v>205</v>
       </c>
-      <c r="C38" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D38" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E38" s="85" t="s">
+      <c r="C38" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A39" s="84" t="s">
+    <row r="39" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A39" s="80" t="s">
         <v>206</v>
       </c>
-      <c r="B39" s="84" t="s">
+      <c r="B39" s="80" t="s">
         <v>207</v>
       </c>
-      <c r="C39" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D39" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" s="85" t="s">
+      <c r="C39" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A40" s="84" t="s">
+    <row r="40" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A40" s="80" t="s">
         <v>208</v>
       </c>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="80" t="s">
         <v>209</v>
       </c>
-      <c r="C40" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E40" s="85" t="s">
+      <c r="C40" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A41" s="84" t="s">
+    <row r="41" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A41" s="80" t="s">
         <v>210</v>
       </c>
-      <c r="B41" s="84" t="s">
+      <c r="B41" s="80" t="s">
         <v>211</v>
       </c>
-      <c r="C41" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="85" t="s">
+      <c r="C41" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E41" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="42" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A42" s="84" t="s">
+    <row r="42" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A42" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="B42" s="84" t="s">
+      <c r="B42" s="80" t="s">
         <v>213</v>
       </c>
-      <c r="C42" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" s="85" t="s">
+      <c r="C42" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="43" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A43" s="84" t="s">
+    <row r="43" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A43" s="80" t="s">
         <v>214</v>
       </c>
-      <c r="B43" s="84" t="s">
+      <c r="B43" s="80" t="s">
         <v>215</v>
       </c>
-      <c r="C43" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="85" t="s">
+      <c r="C43" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E43" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A44" s="84" t="s">
+    <row r="44" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A44" s="80" t="s">
         <v>216</v>
       </c>
-      <c r="B44" s="84" t="s">
+      <c r="B44" s="80" t="s">
         <v>217</v>
       </c>
-      <c r="C44" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D44" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E44" s="85" t="s">
+      <c r="C44" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="45" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A45" s="84" t="s">
+    <row r="45" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A45" s="80" t="s">
         <v>218</v>
       </c>
-      <c r="B45" s="84" t="s">
+      <c r="B45" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="C45" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D45" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E45" s="85" t="s">
+      <c r="C45" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="46" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A46" s="84" t="s">
+    <row r="46" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A46" s="80" t="s">
         <v>220</v>
       </c>
-      <c r="B46" s="84" t="s">
+      <c r="B46" s="80" t="s">
         <v>221</v>
       </c>
-      <c r="C46" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D46" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E46" s="85" t="s">
+      <c r="C46" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A47" s="84" t="s">
+    <row r="47" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A47" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="B47" s="84" t="s">
+      <c r="B47" s="80" t="s">
         <v>223</v>
       </c>
-      <c r="C47" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D47" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E47" s="85" t="s">
+      <c r="C47" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E47" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="48" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A48" s="84" t="s">
+    <row r="48" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A48" s="80" t="s">
         <v>224</v>
       </c>
-      <c r="B48" s="84" t="s">
+      <c r="B48" s="80" t="s">
         <v>225</v>
       </c>
-      <c r="C48" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D48" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E48" s="85" t="s">
+      <c r="C48" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E48" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A49" s="84" t="s">
+    <row r="49" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A49" s="80" t="s">
         <v>226</v>
       </c>
-      <c r="B49" s="84" t="s">
+      <c r="B49" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="C49" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E49" s="85" t="s">
+      <c r="C49" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="50" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A50" s="84" t="s">
+    <row r="50" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A50" s="80" t="s">
         <v>228</v>
       </c>
-      <c r="B50" s="84" t="s">
+      <c r="B50" s="80" t="s">
         <v>229</v>
       </c>
-      <c r="C50" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D50" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E50" s="85" t="s">
+      <c r="C50" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E50" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="51" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A51" s="84" t="s">
+    <row r="51" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A51" s="80" t="s">
         <v>230</v>
       </c>
-      <c r="B51" s="84" t="s">
+      <c r="B51" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="C51" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D51" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E51" s="85" t="s">
+      <c r="C51" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D51" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E51" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="52" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A52" s="84" t="s">
+    <row r="52" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A52" s="80" t="s">
         <v>232</v>
       </c>
-      <c r="B52" s="84" t="s">
+      <c r="B52" s="80" t="s">
         <v>233</v>
       </c>
-      <c r="C52" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E52" s="85" t="s">
+      <c r="C52" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E52" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="53" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A53" s="84" t="s">
+    <row r="53" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A53" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="B53" s="84" t="s">
+      <c r="B53" s="80" t="s">
         <v>235</v>
       </c>
-      <c r="C53" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D53" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E53" s="85" t="s">
+      <c r="C53" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E53" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="54" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A54" s="84" t="s">
+    <row r="54" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A54" s="80" t="s">
         <v>236</v>
       </c>
-      <c r="B54" s="84" t="s">
+      <c r="B54" s="80" t="s">
         <v>237</v>
       </c>
-      <c r="C54" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E54" s="85" t="s">
+      <c r="C54" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E54" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="55" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A55" s="84" t="s">
+    <row r="55" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A55" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="B55" s="84" t="s">
+      <c r="B55" s="80" t="s">
         <v>239</v>
       </c>
-      <c r="C55" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D55" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E55" s="85" t="s">
+      <c r="C55" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E55" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="56" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A56" s="84" t="s">
+    <row r="56" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A56" s="80" t="s">
         <v>240</v>
       </c>
-      <c r="B56" s="84" t="s">
+      <c r="B56" s="80" t="s">
         <v>241</v>
       </c>
-      <c r="C56" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D56" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E56" s="85" t="s">
+      <c r="C56" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E56" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="57" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A57" s="84" t="s">
+    <row r="57" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A57" s="80" t="s">
         <v>242</v>
       </c>
-      <c r="B57" s="84" t="s">
+      <c r="B57" s="80" t="s">
         <v>243</v>
       </c>
-      <c r="C57" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E57" s="85" t="s">
+      <c r="C57" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="58" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A58" s="84" t="s">
+    <row r="58" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A58" s="80" t="s">
         <v>244</v>
       </c>
-      <c r="B58" s="84" t="s">
+      <c r="B58" s="80" t="s">
         <v>245</v>
       </c>
-      <c r="C58" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E58" s="85" t="s">
+      <c r="C58" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E58" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="59" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A59" s="86" t="s">
+    <row r="59" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A59" s="84" t="s">
         <v>246</v>
       </c>
-      <c r="B59" s="86" t="s">
+      <c r="B59" s="84" t="s">
         <v>247</v>
       </c>
-      <c r="C59" s="86" t="s">
+      <c r="C59" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="86" t="s">
+      <c r="D59" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E59" s="87" t="s">
+      <c r="E59" s="85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A60" s="83" t="s">
+    <row r="60" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A60" s="82" t="s">
         <v>248</v>
       </c>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84"/>
-      <c r="D60" s="84"/>
-      <c r="E60" s="85"/>
-    </row>
-    <row r="61" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A61" s="84" t="s">
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="83"/>
+    </row>
+    <row r="61" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A61" s="80" t="s">
         <v>249</v>
       </c>
-      <c r="B61" s="84" t="s">
+      <c r="B61" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="C61" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D61" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E61" s="85" t="s">
+      <c r="C61" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="83" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="62" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A62" s="84" t="s">
+    <row r="62" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A62" s="80" t="s">
         <v>250</v>
       </c>
-      <c r="B62" s="84" t="s">
+      <c r="B62" s="80" t="s">
         <v>194</v>
       </c>
-      <c r="C62" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D62" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E62" s="85" t="s">
+      <c r="C62" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E62" s="83" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="63" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A63" s="84" t="s">
+    <row r="63" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A63" s="80" t="s">
         <v>251</v>
       </c>
-      <c r="B63" s="84" t="s">
+      <c r="B63" s="80" t="s">
         <v>252</v>
       </c>
-      <c r="C63" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D63" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E63" s="85" t="s">
+      <c r="C63" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="64" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A64" s="84" t="s">
+    <row r="64" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A64" s="80" t="s">
         <v>253</v>
       </c>
-      <c r="B64" s="84" t="s">
+      <c r="B64" s="80" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D64" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E64" s="85" t="s">
+      <c r="C64" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D64" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="65" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A65" s="84" t="s">
+    <row r="65" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A65" s="80" t="s">
         <v>254</v>
       </c>
-      <c r="B65" s="84" t="s">
+      <c r="B65" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="C65" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D65" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E65" s="85" t="s">
+      <c r="C65" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E65" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="66" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A66" s="84" t="s">
+    <row r="66" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A66" s="80" t="s">
         <v>255</v>
       </c>
-      <c r="B66" s="84" t="s">
+      <c r="B66" s="80" t="s">
         <v>203</v>
       </c>
-      <c r="C66" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D66" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E66" s="85" t="s">
+      <c r="C66" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D66" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E66" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="67" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A67" s="84" t="s">
+    <row r="67" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A67" s="80" t="s">
         <v>256</v>
       </c>
-      <c r="B67" s="84" t="s">
+      <c r="B67" s="80" t="s">
         <v>205</v>
       </c>
-      <c r="C67" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D67" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E67" s="85" t="s">
+      <c r="C67" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D67" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E67" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="68" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A68" s="84" t="s">
+    <row r="68" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A68" s="80" t="s">
         <v>257</v>
       </c>
-      <c r="B68" s="84" t="s">
+      <c r="B68" s="80" t="s">
         <v>207</v>
       </c>
-      <c r="C68" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D68" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E68" s="85" t="s">
+      <c r="C68" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E68" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="69" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A69" s="84" t="s">
+    <row r="69" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A69" s="80" t="s">
         <v>258</v>
       </c>
-      <c r="B69" s="84" t="s">
+      <c r="B69" s="80" t="s">
         <v>209</v>
       </c>
-      <c r="C69" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D69" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E69" s="85" t="s">
+      <c r="C69" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E69" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="70" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A70" s="84" t="s">
+    <row r="70" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A70" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="B70" s="84" t="s">
+      <c r="B70" s="80" t="s">
         <v>211</v>
       </c>
-      <c r="C70" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D70" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E70" s="85" t="s">
+      <c r="C70" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E70" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="71" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A71" s="84" t="s">
+    <row r="71" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A71" s="80" t="s">
         <v>260</v>
       </c>
-      <c r="B71" s="84" t="s">
+      <c r="B71" s="80" t="s">
         <v>213</v>
       </c>
-      <c r="C71" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D71" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E71" s="85" t="s">
+      <c r="C71" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D71" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A72" s="84" t="s">
+    <row r="72" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A72" s="80" t="s">
         <v>261</v>
       </c>
-      <c r="B72" s="84" t="s">
+      <c r="B72" s="80" t="s">
         <v>215</v>
       </c>
-      <c r="C72" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D72" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E72" s="85" t="s">
+      <c r="C72" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D72" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E72" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="73" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A73" s="84" t="s">
+    <row r="73" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A73" s="80" t="s">
         <v>262</v>
       </c>
-      <c r="B73" s="84" t="s">
+      <c r="B73" s="80" t="s">
         <v>217</v>
       </c>
-      <c r="C73" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D73" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E73" s="85" t="s">
+      <c r="C73" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E73" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="74" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A74" s="84" t="s">
+    <row r="74" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A74" s="80" t="s">
         <v>263</v>
       </c>
-      <c r="B74" s="84" t="s">
+      <c r="B74" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="C74" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E74" s="85" t="s">
+      <c r="C74" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="75" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A75" s="84" t="s">
+    <row r="75" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A75" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="B75" s="84" t="s">
+      <c r="B75" s="80" t="s">
         <v>221</v>
       </c>
-      <c r="C75" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D75" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E75" s="85" t="s">
+      <c r="C75" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D75" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="76" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A76" s="84" t="s">
+    <row r="76" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A76" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="B76" s="84" t="s">
+      <c r="B76" s="80" t="s">
         <v>223</v>
       </c>
-      <c r="C76" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D76" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E76" s="85" t="s">
+      <c r="C76" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D76" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E76" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="77" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A77" s="84" t="s">
+    <row r="77" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A77" s="80" t="s">
         <v>266</v>
       </c>
-      <c r="B77" s="84" t="s">
+      <c r="B77" s="80" t="s">
         <v>225</v>
       </c>
-      <c r="C77" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D77" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E77" s="85" t="s">
+      <c r="C77" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D77" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="78" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A78" s="84" t="s">
+    <row r="78" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A78" s="80" t="s">
         <v>267</v>
       </c>
-      <c r="B78" s="84" t="s">
+      <c r="B78" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="C78" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D78" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E78" s="85" t="s">
+      <c r="C78" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D78" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E78" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="79" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A79" s="84" t="s">
+    <row r="79" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A79" s="80" t="s">
         <v>268</v>
       </c>
-      <c r="B79" s="84" t="s">
+      <c r="B79" s="80" t="s">
         <v>229</v>
       </c>
-      <c r="C79" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D79" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E79" s="85" t="s">
+      <c r="C79" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D79" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E79" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="80" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A80" s="84" t="s">
+    <row r="80" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A80" s="80" t="s">
         <v>269</v>
       </c>
-      <c r="B80" s="84" t="s">
+      <c r="B80" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="C80" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D80" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E80" s="85" t="s">
+      <c r="C80" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E80" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A81" s="84" t="s">
+    <row r="81" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A81" s="80" t="s">
         <v>270</v>
       </c>
-      <c r="B81" s="84" t="s">
+      <c r="B81" s="80" t="s">
         <v>233</v>
       </c>
-      <c r="C81" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D81" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E81" s="85" t="s">
+      <c r="C81" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D81" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E81" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="82" s="82" customFormat="1" ht="16" customHeight="1" spans="1:9">
-      <c r="A82" s="84" t="s">
+    <row r="82" s="76" customFormat="1" ht="16" customHeight="1" spans="1:9">
+      <c r="A82" s="80" t="s">
         <v>271</v>
       </c>
-      <c r="B82" s="84" t="s">
+      <c r="B82" s="80" t="s">
         <v>235</v>
       </c>
-      <c r="C82" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D82" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E82" s="85" t="s">
+      <c r="C82" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D82" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E82" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="I82" s="82">
+      <c r="I82" s="76">
         <f>SUM(B79)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A83" s="84" t="s">
+    <row r="83" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A83" s="80" t="s">
         <v>272</v>
       </c>
-      <c r="B83" s="84" t="s">
+      <c r="B83" s="80" t="s">
         <v>237</v>
       </c>
-      <c r="C83" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D83" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E83" s="85" t="s">
+      <c r="C83" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D83" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E83" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="84" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A84" s="84" t="s">
+    <row r="84" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A84" s="80" t="s">
         <v>273</v>
       </c>
-      <c r="B84" s="84" t="s">
+      <c r="B84" s="80" t="s">
         <v>239</v>
       </c>
-      <c r="C84" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D84" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E84" s="85" t="s">
+      <c r="C84" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D84" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E84" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="85" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A85" s="84" t="s">
+    <row r="85" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A85" s="80" t="s">
         <v>274</v>
       </c>
-      <c r="B85" s="84" t="s">
+      <c r="B85" s="80" t="s">
         <v>241</v>
       </c>
-      <c r="C85" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E85" s="85" t="s">
+      <c r="C85" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D85" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E85" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="86" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A86" s="84" t="s">
+    <row r="86" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A86" s="80" t="s">
         <v>275</v>
       </c>
-      <c r="B86" s="84" t="s">
+      <c r="B86" s="80" t="s">
         <v>243</v>
       </c>
-      <c r="C86" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D86" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E86" s="85" t="s">
+      <c r="C86" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D86" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E86" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="87" s="82" customFormat="1" ht="16" customHeight="1" spans="1:5">
-      <c r="A87" s="84" t="s">
+    <row r="87" s="76" customFormat="1" ht="16" customHeight="1" spans="1:5">
+      <c r="A87" s="80" t="s">
         <v>276</v>
       </c>
-      <c r="B87" s="84" t="s">
+      <c r="B87" s="80" t="s">
         <v>245</v>
       </c>
-      <c r="C87" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="D87" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="E87" s="85" t="s">
+      <c r="C87" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D87" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="E87" s="83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="88" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A88" s="86" t="s">
+    <row r="88" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A88" s="84" t="s">
         <v>277</v>
       </c>
-      <c r="B88" s="86" t="s">
+      <c r="B88" s="84" t="s">
         <v>247</v>
       </c>
-      <c r="C88" s="86" t="s">
+      <c r="C88" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D88" s="86" t="s">
+      <c r="D88" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E88" s="87" t="s">
+      <c r="E88" s="85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="89" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A89" s="83" t="s">
+    <row r="89" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A89" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="B89" s="84"/>
-      <c r="C89" s="84"/>
-      <c r="D89" s="84"/>
-      <c r="E89" s="85"/>
-    </row>
-    <row r="90" s="82" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A90" s="86" t="s">
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="80"/>
+      <c r="E89" s="83"/>
+    </row>
+    <row r="90" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A90" s="84" t="s">
         <v>185</v>
       </c>
-      <c r="B90" s="86" t="s">
+      <c r="B90" s="84" t="s">
         <v>278</v>
       </c>
-      <c r="C90" s="86" t="s">
+      <c r="C90" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="D90" s="86" t="s">
+      <c r="D90" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="E90" s="87" t="s">
+      <c r="E90" s="85" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="91" customFormat="1" spans="4:9">
-      <c r="D91" s="88"/>
-      <c r="E91" s="88"/>
-      <c r="F91" s="88"/>
-      <c r="G91" s="89"/>
-      <c r="H91" s="88"/>
-      <c r="I91" s="89"/>
+      <c r="D91" s="86"/>
+      <c r="E91" s="86"/>
+      <c r="F91" s="86"/>
+      <c r="G91" s="87"/>
+      <c r="H91" s="86"/>
+      <c r="I91" s="87"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="89" t="s">
+      <c r="A92" s="87" t="s">
         <v>279</v>
       </c>
-      <c r="B92" s="88" t="s">
+      <c r="B92" s="86" t="s">
         <v>280</v>
       </c>
-      <c r="C92" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D92" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E92" s="88" t="s">
+      <c r="C92" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D92" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E92" s="86" t="s">
         <v>281</v>
       </c>
-      <c r="F92" s="88"/>
-      <c r="G92" s="89"/>
-      <c r="H92" s="88"/>
-      <c r="I92" s="89"/>
+      <c r="F92" s="86"/>
+      <c r="G92" s="87"/>
+      <c r="H92" s="86"/>
+      <c r="I92" s="87"/>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>282</v>
       </c>
-      <c r="B93" s="88" t="s">
+      <c r="B93" s="86" t="s">
         <v>283</v>
       </c>
-      <c r="C93" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D93" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E93" s="88" t="s">
+      <c r="C93" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D93" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E93" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="F93" s="88"/>
-      <c r="G93" s="89"/>
-      <c r="H93" s="88"/>
-      <c r="I93" s="89"/>
+      <c r="F93" s="86"/>
+      <c r="G93" s="87"/>
+      <c r="H93" s="86"/>
+      <c r="I93" s="87"/>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>284</v>
       </c>
-      <c r="B94" s="88" t="s">
+      <c r="B94" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="C94" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D94" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E94" s="88" t="s">
+      <c r="C94" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D94" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E94" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F94" s="88"/>
-      <c r="G94" s="89"/>
-      <c r="H94" s="88"/>
-      <c r="I94" s="89"/>
+      <c r="F94" s="86"/>
+      <c r="G94" s="87"/>
+      <c r="H94" s="86"/>
+      <c r="I94" s="87"/>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>287</v>
       </c>
-      <c r="B95" s="88" t="s">
+      <c r="B95" s="86" t="s">
         <v>288</v>
       </c>
-      <c r="C95" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D95" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E95" s="88" t="s">
+      <c r="C95" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D95" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E95" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F95" s="88"/>
-      <c r="G95" s="89"/>
-      <c r="H95" s="88"/>
-      <c r="I95" s="89"/>
+      <c r="F95" s="86"/>
+      <c r="G95" s="87"/>
+      <c r="H95" s="86"/>
+      <c r="I95" s="87"/>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>289</v>
       </c>
-      <c r="B96" s="88" t="s">
+      <c r="B96" s="86" t="s">
         <v>290</v>
       </c>
-      <c r="C96" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D96" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E96" s="88" t="s">
+      <c r="C96" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D96" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E96" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F96" s="88"/>
-      <c r="G96" s="89"/>
-      <c r="H96" s="88"/>
-      <c r="I96" s="89"/>
+      <c r="F96" s="86"/>
+      <c r="G96" s="87"/>
+      <c r="H96" s="86"/>
+      <c r="I96" s="87"/>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>291</v>
       </c>
-      <c r="B97" s="88" t="s">
+      <c r="B97" s="86" t="s">
         <v>292</v>
       </c>
-      <c r="C97" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D97" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E97" s="88" t="s">
+      <c r="C97" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D97" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E97" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F97" s="88"/>
-      <c r="G97" s="89"/>
-      <c r="H97" s="88"/>
-      <c r="I97" s="89"/>
+      <c r="F97" s="86"/>
+      <c r="G97" s="87"/>
+      <c r="H97" s="86"/>
+      <c r="I97" s="87"/>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>293</v>
       </c>
-      <c r="B98" s="88" t="s">
+      <c r="B98" s="86" t="s">
         <v>294</v>
       </c>
-      <c r="C98" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D98" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E98" s="88" t="s">
+      <c r="C98" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D98" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E98" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F98" s="88"/>
-      <c r="G98" s="89"/>
-      <c r="H98" s="88"/>
-      <c r="I98" s="89"/>
+      <c r="F98" s="86"/>
+      <c r="G98" s="87"/>
+      <c r="H98" s="86"/>
+      <c r="I98" s="87"/>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>295</v>
       </c>
-      <c r="B99" s="88" t="s">
+      <c r="B99" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="C99" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D99" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E99" s="88" t="s">
+      <c r="C99" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D99" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E99" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F99" s="88"/>
-      <c r="G99" s="89"/>
-      <c r="H99" s="88"/>
-      <c r="I99" s="89"/>
+      <c r="F99" s="86"/>
+      <c r="G99" s="87"/>
+      <c r="H99" s="86"/>
+      <c r="I99" s="87"/>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>297</v>
       </c>
-      <c r="B100" s="88" t="s">
+      <c r="B100" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C100" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D100" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E100" s="88" t="s">
+      <c r="C100" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D100" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E100" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F100" s="88"/>
-      <c r="G100" s="89"/>
-      <c r="H100" s="88"/>
-      <c r="I100" s="89"/>
+      <c r="F100" s="86"/>
+      <c r="G100" s="87"/>
+      <c r="H100" s="86"/>
+      <c r="I100" s="87"/>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>299</v>
       </c>
-      <c r="B101" s="88" t="s">
+      <c r="B101" s="86" t="s">
         <v>300</v>
       </c>
-      <c r="C101" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D101" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E101" s="88" t="s">
+      <c r="C101" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D101" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E101" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F101" s="88"/>
-      <c r="G101" s="89"/>
-      <c r="H101" s="88"/>
-      <c r="I101" s="89"/>
+      <c r="F101" s="86"/>
+      <c r="G101" s="87"/>
+      <c r="H101" s="86"/>
+      <c r="I101" s="87"/>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>301</v>
       </c>
-      <c r="B102" s="88" t="s">
+      <c r="B102" s="86" t="s">
         <v>302</v>
       </c>
-      <c r="C102" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D102" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E102" s="88" t="s">
+      <c r="C102" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D102" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E102" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F102" s="88"/>
-      <c r="G102" s="89"/>
-      <c r="H102" s="88"/>
-      <c r="I102" s="89"/>
+      <c r="F102" s="86"/>
+      <c r="G102" s="87"/>
+      <c r="H102" s="86"/>
+      <c r="I102" s="87"/>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>303</v>
       </c>
-      <c r="B103" s="88" t="s">
+      <c r="B103" s="86" t="s">
         <v>304</v>
       </c>
-      <c r="C103" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D103" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E103" s="88" t="s">
+      <c r="C103" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D103" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E103" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F103" s="88"/>
-      <c r="G103" s="89"/>
-      <c r="H103" s="88"/>
-      <c r="I103" s="89"/>
+      <c r="F103" s="86"/>
+      <c r="G103" s="87"/>
+      <c r="H103" s="86"/>
+      <c r="I103" s="87"/>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>305</v>
       </c>
-      <c r="B104" s="88" t="s">
+      <c r="B104" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="C104" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D104" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E104" s="88" t="s">
+      <c r="C104" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D104" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E104" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F104" s="88"/>
-      <c r="G104" s="89"/>
-      <c r="H104" s="88"/>
-      <c r="I104" s="89"/>
+      <c r="F104" s="86"/>
+      <c r="G104" s="87"/>
+      <c r="H104" s="86"/>
+      <c r="I104" s="87"/>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>307</v>
       </c>
-      <c r="B105" s="88" t="s">
+      <c r="B105" s="86" t="s">
         <v>308</v>
       </c>
-      <c r="C105" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D105" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E105" s="88" t="s">
+      <c r="C105" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D105" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E105" s="86" t="s">
         <v>159</v>
       </c>
-      <c r="F105" s="88"/>
-      <c r="G105" s="89"/>
-      <c r="H105" s="88"/>
-      <c r="I105" s="89"/>
+      <c r="F105" s="86"/>
+      <c r="G105" s="87"/>
+      <c r="H105" s="86"/>
+      <c r="I105" s="87"/>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>309</v>
       </c>
-      <c r="B106" s="88" t="s">
+      <c r="B106" s="86" t="s">
         <v>310</v>
       </c>
-      <c r="C106" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D106" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E106" s="88" t="s">
+      <c r="C106" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D106" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E106" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F106" s="88"/>
-      <c r="G106" s="89"/>
-      <c r="H106" s="88"/>
-      <c r="I106" s="89"/>
+      <c r="F106" s="86"/>
+      <c r="G106" s="87"/>
+      <c r="H106" s="86"/>
+      <c r="I106" s="87"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>312</v>
       </c>
-      <c r="B107" s="88" t="s">
+      <c r="B107" s="86" t="s">
         <v>313</v>
       </c>
-      <c r="C107" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D107" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E107" s="88" t="s">
+      <c r="C107" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D107" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E107" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F107" s="88"/>
-      <c r="G107" s="89"/>
-      <c r="H107" s="88"/>
-      <c r="I107" s="89"/>
+      <c r="F107" s="86"/>
+      <c r="G107" s="87"/>
+      <c r="H107" s="86"/>
+      <c r="I107" s="87"/>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>314</v>
       </c>
-      <c r="B108" s="88" t="s">
+      <c r="B108" s="86" t="s">
         <v>315</v>
       </c>
-      <c r="C108" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D108" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E108" s="88" t="s">
+      <c r="C108" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D108" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E108" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F108" s="88"/>
-      <c r="G108" s="89"/>
-      <c r="H108" s="88"/>
-      <c r="I108" s="89"/>
+      <c r="F108" s="86"/>
+      <c r="G108" s="87"/>
+      <c r="H108" s="86"/>
+      <c r="I108" s="87"/>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>316</v>
       </c>
-      <c r="B109" s="88" t="s">
+      <c r="B109" s="86" t="s">
         <v>317</v>
       </c>
-      <c r="C109" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D109" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E109" s="88" t="s">
+      <c r="C109" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D109" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E109" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F109" s="88"/>
-      <c r="G109" s="89"/>
-      <c r="H109" s="88"/>
-      <c r="I109" s="89"/>
+      <c r="F109" s="86"/>
+      <c r="G109" s="87"/>
+      <c r="H109" s="86"/>
+      <c r="I109" s="87"/>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>318</v>
       </c>
-      <c r="B110" s="88" t="s">
+      <c r="B110" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="C110" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D110" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E110" s="88" t="s">
+      <c r="C110" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D110" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E110" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F110" s="88"/>
-      <c r="G110" s="89"/>
-      <c r="H110" s="88"/>
-      <c r="I110" s="89"/>
+      <c r="F110" s="86"/>
+      <c r="G110" s="87"/>
+      <c r="H110" s="86"/>
+      <c r="I110" s="87"/>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>320</v>
       </c>
-      <c r="B111" s="88" t="s">
+      <c r="B111" s="86" t="s">
         <v>321</v>
       </c>
-      <c r="C111" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D111" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E111" s="88" t="s">
+      <c r="C111" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D111" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E111" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F111" s="88"/>
-      <c r="G111" s="89"/>
-      <c r="H111" s="88"/>
-      <c r="I111" s="89"/>
+      <c r="F111" s="86"/>
+      <c r="G111" s="87"/>
+      <c r="H111" s="86"/>
+      <c r="I111" s="87"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>322</v>
       </c>
-      <c r="B112" s="88" t="s">
+      <c r="B112" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C112" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D112" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E112" s="88" t="s">
+      <c r="C112" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D112" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E112" s="86" t="s">
         <v>311</v>
       </c>
-      <c r="F112" s="88"/>
-      <c r="G112" s="89"/>
-      <c r="H112" s="88"/>
-      <c r="I112" s="89"/>
+      <c r="F112" s="86"/>
+      <c r="G112" s="87"/>
+      <c r="H112" s="86"/>
+      <c r="I112" s="87"/>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>324</v>
       </c>
-      <c r="B113" s="88" t="s">
+      <c r="B113" s="86" t="s">
         <v>325</v>
       </c>
-      <c r="C113" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D113" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E113" s="88" t="s">
+      <c r="C113" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D113" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E113" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="F113" s="88"/>
-      <c r="G113" s="89"/>
-      <c r="H113" s="88"/>
-      <c r="I113" s="89"/>
+      <c r="F113" s="86"/>
+      <c r="G113" s="87"/>
+      <c r="H113" s="86"/>
+      <c r="I113" s="87"/>
     </row>
     <row r="114" ht="24" spans="1:9">
       <c r="A114" t="s">
         <v>326</v>
       </c>
-      <c r="B114" s="88" t="s">
+      <c r="B114" s="86" t="s">
         <v>327</v>
       </c>
-      <c r="C114" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D114" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E114" s="88" t="s">
+      <c r="C114" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D114" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E114" s="86" t="s">
         <v>328</v>
       </c>
-      <c r="F114" s="88"/>
-      <c r="G114" s="89"/>
-      <c r="H114" s="88"/>
-      <c r="I114" s="89"/>
+      <c r="F114" s="86"/>
+      <c r="G114" s="87"/>
+      <c r="H114" s="86"/>
+      <c r="I114" s="87"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>329</v>
       </c>
-      <c r="B115" s="88" t="s">
+      <c r="B115" s="86" t="s">
         <v>330</v>
       </c>
-      <c r="C115" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="D115" s="90" t="s">
-        <v>154</v>
-      </c>
-      <c r="E115" s="88" t="s">
+      <c r="C115" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="D115" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="E115" s="86" t="s">
         <v>331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: add zhong xin scan equipment
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
+++ b/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="504"/>
+    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="504" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="secs指令" sheetId="2" r:id="rId1"/>
@@ -1891,6 +1891,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color rgb="FF4472C4"/>
       <name val="Calibri"/>
@@ -1907,13 +1914,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="42">
@@ -3927,7 +3927,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
@@ -4894,7 +4894,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18:C22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -5505,10 +5505,10 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
feature: zhong che yixing new version
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
+++ b/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="504" activeTab="3"/>
+    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="504"/>
   </bookViews>
   <sheets>
     <sheet name="secs指令" sheetId="2" r:id="rId1"/>
@@ -113,7 +113,7 @@
   <si>
     <t>报警/解除报警上报给Host
 alarm_code的数据类型：BINARRY
-alarm_id的数据类型：I4
+alarm_id的数据类型：U4
 alarm_text的数据类型：ASCII</t>
   </si>
   <si>
@@ -1891,13 +1891,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF4472C4"/>
       <name val="Calibri"/>
@@ -1914,6 +1907,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="42">
@@ -3927,10 +3927,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -4894,7 +4894,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -5505,10 +5505,10 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
feature: complete zhong che yi xing
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
+++ b/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
@@ -2961,8 +2961,8 @@
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3868420</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>147</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
@@ -3004,7 +3004,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2091690</xdr:colOff>
+      <xdr:colOff>2672715</xdr:colOff>
       <xdr:row>161</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
@@ -3046,7 +3046,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3395345</xdr:colOff>
+      <xdr:colOff>3976370</xdr:colOff>
       <xdr:row>180</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -3088,7 +3088,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3357245</xdr:colOff>
+      <xdr:colOff>3938270</xdr:colOff>
       <xdr:row>209</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
@@ -3130,7 +3130,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2042795</xdr:colOff>
+      <xdr:colOff>2623820</xdr:colOff>
       <xdr:row>231</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -3172,7 +3172,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2065020</xdr:colOff>
+      <xdr:colOff>2646045</xdr:colOff>
       <xdr:row>258</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
@@ -3214,7 +3214,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1965960</xdr:colOff>
+      <xdr:colOff>2546985</xdr:colOff>
       <xdr:row>289</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
@@ -3256,7 +3256,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1927860</xdr:colOff>
+      <xdr:colOff>2508885</xdr:colOff>
       <xdr:row>319</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
@@ -3298,7 +3298,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1935480</xdr:colOff>
+      <xdr:colOff>2516505</xdr:colOff>
       <xdr:row>345</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3340,7 +3340,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1874520</xdr:colOff>
+      <xdr:colOff>2455545</xdr:colOff>
       <xdr:row>376</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
@@ -3382,7 +3382,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1889760</xdr:colOff>
+      <xdr:colOff>2470785</xdr:colOff>
       <xdr:row>407</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -3424,7 +3424,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3144520</xdr:colOff>
+      <xdr:colOff>3725545</xdr:colOff>
       <xdr:row>411</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -3992,7 +3992,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4552,9 +4552,9 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="4"/>
@@ -4847,7 +4847,7 @@
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -4916,12 +4916,12 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="106.5" customWidth="1"/>
+    <col min="1" max="1" width="98.875" customWidth="1"/>
     <col min="2" max="2" width="54.8916666666667" customWidth="1"/>
     <col min="3" max="3" width="5.95" customWidth="1"/>
     <col min="4" max="4" width="14.325" customWidth="1"/>

</xml_diff>

<commit_message>
feature: zhong che yi xing complete
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
+++ b/equipment_cyg/product/zhong_che_yi_xing/zhong_che_yi_xing_manual.xlsx
@@ -1741,6 +1741,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color rgb="FF4472C4"/>
       <name val="Calibri"/>
@@ -1757,13 +1764,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="42">
@@ -4914,9 +4914,9 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>